<commit_message>
fix quote template liability
</commit_message>
<xml_diff>
--- a/lib/quote_template.xlsx
+++ b/lib/quote_template.xlsx
@@ -470,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -647,11 +647,11 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
+      <left>
+        <color indexed="0"/>
       </left>
-      <right>
-        <color indexed="0"/>
+      <right style="thin">
+        <color indexed="8"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -667,53 +667,11 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top style="thin">
-        <color indexed="8"/>
+      <top>
+        <color indexed="0"/>
       </top>
       <bottom>
         <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
       </bottom>
     </border>
     <border>
@@ -767,7 +725,7 @@
       <protection/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment/>
     </xf>
@@ -943,10 +901,6 @@
       <alignment horizontal="center"/>
       <protection/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="13" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="12" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
@@ -959,11 +913,7 @@
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
@@ -983,12 +933,8 @@
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
       <protection/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -999,11 +945,7 @@
       <alignment horizontal="right"/>
       <protection/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="21" applyFont="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="17" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="21" applyFont="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
@@ -1023,7 +965,7 @@
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="21" applyFont="1" applyBorder="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="21" applyFont="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
@@ -1582,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A21">
+      <selection pane="topLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2278,19 +2220,19 @@
       <c r="R33" s="9"/>
     </row>
     <row r="34" spans="1:18" ht="15" customHeight="1">
-      <c r="A34" s="44"/>
-      <c r="B34" s="45" t="s">
+      <c r="A34" s="44" t="s">
         <v>25</v>
       </c>
+      <c r="B34" s="44"/>
       <c r="C34" s="45"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="45" t="s">
+      <c r="D34" s="45"/>
+      <c r="E34" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G34" s="45"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="48"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="47"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
@@ -2302,19 +2244,19 @@
       <c r="R34" s="9"/>
     </row>
     <row r="35" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50" t="s">
+      <c r="A35" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="52" t="s">
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="51"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="54"/>
+      <c r="F35"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="52"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
@@ -2326,19 +2268,19 @@
       <c r="R35" s="9"/>
     </row>
     <row r="36" spans="1:18" ht="15" customHeight="1">
-      <c r="A36" s="55"/>
-      <c r="B36" s="56" t="s">
+      <c r="A36" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51" t="s">
+      <c r="B36" s="50"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="G36" s="51"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="58"/>
+      <c r="F36"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="55"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
@@ -2350,19 +2292,19 @@
       <c r="R36" s="9"/>
     </row>
     <row r="37" spans="1:18" ht="15" customHeight="1">
-      <c r="A37" s="59"/>
-      <c r="B37" s="60" t="s">
+      <c r="A37" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61" t="s">
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="62"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="64"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="60"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
@@ -2374,15 +2316,15 @@
       <c r="R37" s="9"/>
     </row>
     <row r="38" spans="10:18" ht="15" customHeight="1">
-      <c r="J38" s="65"/>
-      <c r="K38" s="65"/>
-      <c r="L38" s="65"/>
-      <c r="M38" s="65"/>
-      <c r="N38" s="65"/>
-      <c r="O38" s="65"/>
-      <c r="P38" s="65"/>
-      <c r="Q38" s="65"/>
-      <c r="R38" s="65"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="61"/>
+      <c r="P38" s="61"/>
+      <c r="Q38" s="61"/>
+      <c r="R38" s="61"/>
     </row>
     <row r="39" ht="16.5" customHeight="1"/>
     <row r="42" ht="15" customHeight="1"/>
@@ -2438,7 +2380,7 @@
     <mergeCell ref="A33:E33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B36" r:id="rId1" display="TBrewer@bigislandgroup.ca"/>
+    <hyperlink ref="A36" r:id="rId1" display="TBrewer@bigislandgroup.ca"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="1"/>

</xml_diff>